<commit_message>
g-index 26. Added mean and media citation to long ES and EN versions
</commit_message>
<xml_diff>
--- a/data/education_en.xlsx
+++ b/data/education_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69160C81-3C6B-4DC7-B85F-D999FBF81D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF6F1D-E97A-499F-A277-B32C69BDD06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="2865" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>what</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Bogota, Colombia</t>
   </si>
   <si>
-    <t>Research project: 4.90/5.00</t>
-  </si>
-  <si>
     <t>Best overall performance in the MSc</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>\href{https://www.stir.ac.uk/}{University of Stirling}</t>
   </si>
   <si>
-    <t>Dissertation \href{https://dspace.stir.ac.uk/handle/1893/21102}{\textbf{\textit{Contextual musicality: vocal modulation and its perception in human social interaction}}}</t>
-  </si>
-  <si>
     <t>Supervisors: \href{https://www.scraigroberts.com/}{Prof. S. Craig Roberts} and \href{https://scholar.google.com/citations?user=iDDoxVsAAAAJ}{Prof. Anthony C. Little}</t>
   </si>
   <si>
@@ -83,6 +77,15 @@
   </si>
   <si>
     <t>\href{https://www.upn.edu.co/}{Universidad Pedagógica Nacional}</t>
+  </si>
+  <si>
+    <t>Research project: \href{https://dspace.stir.ac.uk/handle/1893/21102}{\textbf{\textit{Contextual musicality: vocal modulation and its perception in human social interaction}}}</t>
+  </si>
+  <si>
+    <t>Research project: \textbf{\textit{Variation of pitch and loudness range of human voice in response to intra- and inter-sexual stimuli}}</t>
+  </si>
+  <si>
+    <t>Research project: 4.90/5.00 | \href{https://revistas.pedagogica.edu.co/index.php/revistafba/article/view/50}{\textbf{\textit{El origen no humano de la música}}}</t>
   </si>
 </sst>
 </file>
@@ -633,9 +636,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -673,7 +676,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -779,7 +782,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -921,7 +924,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -929,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,13 +972,13 @@
         <v>2014</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -984,7 +987,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -993,7 +996,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1004,13 +1007,13 @@
         <v>2009</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1019,41 +1022,43 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2006</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -1084,11 +1089,11 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1139,6 +1144,13 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>